<commit_message>
xlsx handle and array creations
</commit_message>
<xml_diff>
--- a/results_file/recurrence.xlsx
+++ b/results_file/recurrence.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
xlsx files adjustments and fixes
</commit_message>
<xml_diff>
--- a/results_file/recurrence.xlsx
+++ b/results_file/recurrence.xlsx
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9">
@@ -502,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13">
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14">
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15">
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18">
@@ -566,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19">
@@ -582,7 +582,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21">
@@ -590,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22">
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23">
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24">
@@ -614,7 +614,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25">
@@ -630,7 +630,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27">
@@ -646,7 +646,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29">
@@ -654,7 +654,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30">
@@ -662,7 +662,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31">
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32">
@@ -678,7 +678,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33">
@@ -686,7 +686,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34">
@@ -702,7 +702,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36">
@@ -710,7 +710,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
@@ -718,7 +718,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38">
@@ -726,7 +726,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39">
@@ -734,7 +734,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40">
@@ -742,7 +742,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41">
@@ -750,7 +750,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42">
@@ -758,7 +758,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43">
@@ -766,7 +766,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44">
@@ -774,7 +774,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45">
@@ -798,7 +798,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48">
@@ -806,7 +806,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49">
@@ -814,7 +814,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50">
@@ -822,7 +822,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51">
@@ -838,7 +838,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53">
@@ -878,7 +878,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58">
@@ -886,7 +886,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59">
@@ -894,7 +894,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60">
@@ -902,7 +902,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61">

</xml_diff>